<commit_message>
Not working backup: log full referenced before assignment in flowchart_no_sensors.py module
</commit_message>
<xml_diff>
--- a/res/report-full.xlsx
+++ b/res/report-full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Building Site PF\PathSolver Server\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\ConcreteFlowchart\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E35D1F-F5C2-4A64-A9C2-2E8C0CE61747}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73492D85-9E7A-4C45-9781-E2C681C667D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="467" windowWidth="16093" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="920" windowWidth="16093" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -477,60 +477,15 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C2">
-        <v>0.19</v>
-      </c>
-      <c r="D2">
-        <v>16.667000000000002</v>
-      </c>
-      <c r="E2">
-        <v>11.333</v>
-      </c>
-      <c r="F2">
-        <v>21.332999999999998</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="C3">
-        <v>0.751</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>21.332999999999998</v>
-      </c>
-      <c r="F3">
-        <v>52</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="C4">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="D4">
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <v>21.332999999999998</v>
-      </c>
-      <c r="F4">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>